<commit_message>
add setup init func; stable v1.1
</commit_message>
<xml_diff>
--- a/data/cases.xlsx
+++ b/data/cases.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065" activeTab="2"/>
+    <workbookView windowWidth="28695" windowHeight="13065" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="smoke" sheetId="2" r:id="rId2"/>
     <sheet name="login" sheetId="3" r:id="rId3"/>
+    <sheet name="setup_init" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="96">
   <si>
     <t>README</t>
   </si>
@@ -311,12 +312,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,29 +327,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,69 +348,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -440,7 +380,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -453,6 +408,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -461,16 +454,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,7 +479,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,49 +593,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,73 +629,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,37 +653,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,17 +682,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -727,37 +715,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,9 +741,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -790,148 +784,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -939,37 +933,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1670,7 +1664,7 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="4"/>
@@ -1681,67 +1675,67 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:23">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -1751,56 +1745,56 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="25.5" spans="1:22">
+    <row r="2" s="1" customFormat="1" spans="1:22">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>72</v>
       </c>
       <c r="V2" s="1">
@@ -1811,67 +1805,61 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="3"/>
+      <c r="P3" s="5"/>
+      <c r="R3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="2"/>
     </row>
     <row r="4" s="1" customFormat="1" spans="1:22">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>79</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1883,27 +1871,22 @@
       <c r="J4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <v>1</v>
       </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="3" t="s">
+      <c r="R4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>85</v>
       </c>
       <c r="V4" s="1" t="s">
@@ -1928,74 +1911,74 @@
   <sheetPr/>
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:23">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -2009,1394 +1992,1369 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:21">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="P3" s="6"/>
-      <c r="R3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="U3" s="3"/>
-    </row>
-    <row r="4" s="2" customFormat="1" spans="1:18">
+      <c r="N3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" s="5"/>
+      <c r="R3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" s="6" customFormat="1" spans="1:18">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="6"/>
+      <c r="P4" s="5"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" s="2" customFormat="1" spans="1:18">
+      <c r="R4" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" s="6" customFormat="1" spans="1:18">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K5" s="1"/>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O5" s="1"/>
-      <c r="P5" s="6"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" s="2" customFormat="1" spans="1:18">
+      <c r="R5" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" s="6" customFormat="1" spans="1:18">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I6" s="1"/>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="6"/>
+      <c r="P6" s="5"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" s="2" customFormat="1" spans="1:18">
+      <c r="R6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" s="6" customFormat="1" spans="1:18">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K7" s="1"/>
-      <c r="L7" s="3" t="s">
+      <c r="L7" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M7" s="1"/>
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="6"/>
+      <c r="P7" s="5"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="1" spans="1:18">
+      <c r="R7" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" s="6" customFormat="1" spans="1:18">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="E8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3" t="s">
+      <c r="H8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" s="2" customFormat="1" spans="1:18">
+      <c r="N8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" s="6" customFormat="1" spans="1:18">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="E9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3" t="s">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O9" s="3"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" s="2" customFormat="1" spans="1:18">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" s="6" customFormat="1" spans="1:18">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="E10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="3" t="s">
+      <c r="N10" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O10" s="1"/>
-      <c r="P10" s="6"/>
+      <c r="P10" s="5"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" s="2" customFormat="1" spans="1:18">
+      <c r="R10" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" s="6" customFormat="1" spans="1:18">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M11" s="1"/>
-      <c r="N11" s="3" t="s">
+      <c r="N11" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O11" s="1"/>
-      <c r="P11" s="6"/>
+      <c r="P11" s="5"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" s="2" customFormat="1" spans="1:18">
+      <c r="R11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" s="6" customFormat="1" spans="1:18">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="E12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K12" s="1"/>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="3" t="s">
+      <c r="N12" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O12" s="1"/>
-      <c r="P12" s="6"/>
+      <c r="P12" s="5"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" s="2" customFormat="1" spans="1:18">
+      <c r="R12" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" s="6" customFormat="1" spans="1:18">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="E13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K13" s="1"/>
-      <c r="L13" s="3" t="s">
+      <c r="L13" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M13" s="1"/>
-      <c r="N13" s="3" t="s">
+      <c r="N13" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O13" s="1"/>
-      <c r="P13" s="6"/>
+      <c r="P13" s="5"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" s="2" customFormat="1" spans="1:18">
+      <c r="R13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" s="6" customFormat="1" spans="1:18">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="E14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M14" s="1"/>
-      <c r="N14" s="3" t="s">
+      <c r="N14" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O14" s="1"/>
-      <c r="P14" s="6"/>
+      <c r="P14" s="5"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" s="2" customFormat="1" spans="1:18">
+      <c r="R14" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" s="6" customFormat="1" spans="1:18">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3" t="s">
+      <c r="H15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" s="2" customFormat="1" spans="1:18">
+      <c r="N15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" s="6" customFormat="1" spans="1:18">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="E16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
+      <c r="H16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3" t="s">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O16" s="3"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" s="2" customFormat="1" spans="1:18">
+      <c r="M16" s="2"/>
+      <c r="N16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" s="6" customFormat="1" spans="1:18">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="E17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I17" s="1"/>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K17" s="1"/>
-      <c r="L17" s="3" t="s">
+      <c r="L17" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M17" s="1"/>
-      <c r="N17" s="3" t="s">
+      <c r="N17" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O17" s="1"/>
-      <c r="P17" s="6"/>
+      <c r="P17" s="5"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" s="2" customFormat="1" spans="1:18">
+      <c r="R17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" s="6" customFormat="1" spans="1:18">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="E18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K18" s="1"/>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M18" s="1"/>
-      <c r="N18" s="3" t="s">
+      <c r="N18" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="P18" s="6"/>
+      <c r="P18" s="5"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" s="2" customFormat="1" spans="1:18">
+      <c r="R18" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" s="6" customFormat="1" spans="1:18">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="3" t="s">
+      <c r="L19" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M19" s="1"/>
-      <c r="N19" s="3" t="s">
+      <c r="N19" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O19" s="1"/>
-      <c r="P19" s="6"/>
+      <c r="P19" s="5"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" s="2" customFormat="1" spans="1:18">
+      <c r="R19" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" s="6" customFormat="1" spans="1:18">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="E20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="N20" s="3" t="s">
+      <c r="N20" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O20" s="1"/>
-      <c r="P20" s="6"/>
+      <c r="P20" s="5"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" s="2" customFormat="1" spans="1:18">
+      <c r="R20" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" s="6" customFormat="1" spans="1:18">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="E21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I21" s="1"/>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K21" s="1"/>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M21" s="1"/>
-      <c r="N21" s="3" t="s">
+      <c r="N21" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="6"/>
+      <c r="P21" s="5"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" s="2" customFormat="1" spans="1:18">
+      <c r="R21" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" s="6" customFormat="1" spans="1:18">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="E22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3" t="s">
+      <c r="H22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2" t="s">
+      <c r="L22" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" s="2" customFormat="1" spans="1:18">
+      <c r="N22" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" s="6" customFormat="1" spans="1:18">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="E23" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3" t="s">
+      <c r="H23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3" t="s">
+      <c r="K23" s="2"/>
+      <c r="L23" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" s="3"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" s="2" customFormat="1" spans="1:18">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" s="6" customFormat="1" spans="1:18">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="3" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="E24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K24" s="1"/>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M24" s="1"/>
-      <c r="N24" s="3" t="s">
+      <c r="N24" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O24" s="1"/>
-      <c r="P24" s="6"/>
+      <c r="P24" s="5"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" s="2" customFormat="1" spans="1:18">
+      <c r="R24" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" s="6" customFormat="1" spans="1:18">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="3" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="3" t="s">
+      <c r="E25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="H25" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I25" s="1"/>
-      <c r="J25" s="3" t="s">
+      <c r="J25" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K25" s="1"/>
-      <c r="L25" s="3" t="s">
+      <c r="L25" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M25" s="1"/>
-      <c r="N25" s="3" t="s">
+      <c r="N25" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O25" s="1"/>
-      <c r="P25" s="6"/>
+      <c r="P25" s="5"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" s="2" customFormat="1" spans="1:18">
+      <c r="R25" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" s="6" customFormat="1" spans="1:18">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="3" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="E26" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="H26" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I26" s="1"/>
-      <c r="J26" s="3" t="s">
+      <c r="J26" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K26" s="1"/>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M26" s="1"/>
-      <c r="N26" s="3" t="s">
+      <c r="N26" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O26" s="1"/>
-      <c r="P26" s="6"/>
+      <c r="P26" s="5"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" s="2" customFormat="1" spans="1:18">
+      <c r="R26" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" s="6" customFormat="1" spans="1:18">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="3" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D27" s="1">
         <v>0</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" s="3" t="s">
+      <c r="E27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="J27" s="3" t="s">
+      <c r="J27" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K27" s="1"/>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M27" s="1"/>
-      <c r="N27" s="3" t="s">
+      <c r="N27" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O27" s="1"/>
-      <c r="P27" s="6"/>
+      <c r="P27" s="5"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" s="2" customFormat="1" spans="1:18">
+      <c r="R27" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" s="6" customFormat="1" spans="1:18">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="3" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" s="3" t="s">
+      <c r="E28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="3" t="s">
+      <c r="J28" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K28" s="1"/>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M28" s="1"/>
-      <c r="N28" s="3" t="s">
+      <c r="N28" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O28" s="1"/>
-      <c r="P28" s="6"/>
+      <c r="P28" s="5"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" s="2" customFormat="1" spans="1:18">
+      <c r="R28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" s="6" customFormat="1" spans="1:18">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D29" s="1">
         <v>0</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="E29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3" t="s">
+      <c r="H29" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2" t="s">
+      <c r="L29" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="M29" s="2"/>
-      <c r="N29" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" s="2" customFormat="1" spans="1:18">
+      <c r="N29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" s="6" customFormat="1" spans="1:18">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="3" t="s">
+      <c r="E30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3" t="s">
+      <c r="H30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3" t="s">
+      <c r="K30" s="2"/>
+      <c r="L30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="O30" s="3"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" s="2" customFormat="1" spans="1:18">
+      <c r="M30" s="2"/>
+      <c r="N30" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" s="6" customFormat="1" spans="1:18">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="3" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="3" t="s">
+      <c r="E31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="3" t="s">
+      <c r="H31" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="3" t="s">
+      <c r="J31" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K31" s="1"/>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M31" s="1"/>
-      <c r="N31" s="3" t="s">
+      <c r="N31" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O31" s="1"/>
-      <c r="P31" s="6"/>
+      <c r="P31" s="5"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" s="2" customFormat="1" spans="1:18">
+      <c r="R31" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" s="6" customFormat="1" spans="1:18">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="3" t="s">
+      <c r="E32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I32" s="1"/>
-      <c r="J32" s="3" t="s">
+      <c r="J32" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M32" s="1"/>
-      <c r="N32" s="3" t="s">
+      <c r="N32" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O32" s="1"/>
-      <c r="P32" s="6"/>
+      <c r="P32" s="5"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" s="2" customFormat="1" spans="1:18">
+      <c r="R32" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" s="6" customFormat="1" spans="1:18">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="3" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="E33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I33" s="1"/>
-      <c r="J33" s="3" t="s">
+      <c r="J33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="K33" s="2"/>
-      <c r="L33" s="3" t="s">
+      <c r="L33" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M33" s="1"/>
-      <c r="N33" s="3" t="s">
+      <c r="N33" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O33" s="1"/>
-      <c r="P33" s="6"/>
+      <c r="P33" s="5"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="34" s="2" customFormat="1" spans="1:18">
+      <c r="R33" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" s="6" customFormat="1" spans="1:18">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G34" s="3" t="s">
+      <c r="E34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H34" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I34" s="1"/>
-      <c r="J34" s="3" t="s">
+      <c r="J34" s="2" t="s">
         <v>88</v>
       </c>
       <c r="K34" s="1"/>
-      <c r="L34" s="3" t="s">
+      <c r="L34" s="2" t="s">
         <v>89</v>
       </c>
       <c r="M34" s="1"/>
-      <c r="N34" s="3" t="s">
+      <c r="N34" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O34" s="1"/>
-      <c r="P34" s="6"/>
+      <c r="P34" s="5"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="3" t="s">
+      <c r="R34" s="2" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3404,42 +3362,42 @@
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G35" s="3" t="s">
+      <c r="E35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="J35" s="3" t="s">
+      <c r="H35" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L35" s="3" t="s">
+      <c r="L35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N35" s="3" t="s">
+      <c r="N35" s="2" t="s">
         <v>68</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="P35" s="6"/>
-      <c r="R35" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="U35" s="3"/>
+      <c r="P35" s="5"/>
+      <c r="R35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3453,4 +3411,133 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:W2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:23">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:21">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="R2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>